<commit_message>
Update bill template and positioned QR code in the right place on it.
</commit_message>
<xml_diff>
--- a/SwissQRBill.xlsx
+++ b/SwissQRBill.xlsx
@@ -2,15 +2,10 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23001"/>
-  <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\erichb\source\repos\SwissQRCodeExcel\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BAEBD92E-1880-4550-8F3D-1C0B7AF3D226}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <workbookPr filterPrivacy="1" checkCompatibility="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46724573-5DA6-4E3A-A9BA-09AAF1239974}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="24496" windowHeight="15796" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15796" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -40,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="17">
   <si>
     <t>Empfangsschein</t>
   </si>
@@ -72,9 +67,6 @@
     <t>Annahmestelle</t>
   </si>
   <si>
-    <t>CH12 3456 7890 1234 5678 9</t>
-  </si>
-  <si>
     <t>John Doe</t>
   </si>
   <si>
@@ -93,7 +85,7 @@
     <t>Datum 05.06.2020</t>
   </si>
   <si>
-    <t>The IBAN entered isn't valid.</t>
+    <t>CH58 0079 1123 0008 8901 2</t>
   </si>
 </sst>
 </file>
@@ -371,13 +363,13 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>21</xdr:row>
-      <xdr:rowOff>90494</xdr:rowOff>
+      <xdr:rowOff>80960</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
       <xdr:colOff>1069950</xdr:colOff>
       <xdr:row>21</xdr:row>
-      <xdr:rowOff>100031</xdr:rowOff>
+      <xdr:rowOff>90497</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -392,7 +384,7 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="0" y="3805244"/>
+          <a:off x="0" y="3795710"/>
           <a:ext cx="2232000" cy="9537"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -424,13 +416,13 @@
       <xdr:col>2</xdr:col>
       <xdr:colOff>1076369</xdr:colOff>
       <xdr:row>21</xdr:row>
-      <xdr:rowOff>100014</xdr:rowOff>
+      <xdr:rowOff>90485</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
       <xdr:colOff>594119</xdr:colOff>
       <xdr:row>21</xdr:row>
-      <xdr:rowOff>109551</xdr:rowOff>
+      <xdr:rowOff>100022</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -445,7 +437,7 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2238419" y="3814764"/>
+          <a:off x="2238419" y="3805235"/>
           <a:ext cx="5328000" cy="9537"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -684,6 +676,56 @@
     </xdr:cxnSp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>1123950</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>79375</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>1058862</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="8" name="Picture 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B1A84A10-63C5-4A08-9FF2-3528FF80C16C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2286000" y="508000"/>
+          <a:ext cx="1778000" cy="1778000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -701,6 +743,7 @@
       <sheetName val="Auswertungen pro Mo"/>
       <sheetName val="Listen"/>
       <sheetName val="Terminvergabe"/>
+      <sheetName val="RECHNUNGSWESEN für QR"/>
     </sheetNames>
     <sheetDataSet>
       <sheetData sheetId="0" refreshError="1"/>
@@ -713,6 +756,7 @@
       <sheetData sheetId="7" refreshError="1"/>
       <sheetData sheetId="8" refreshError="1"/>
       <sheetData sheetId="9" refreshError="1"/>
+      <sheetData sheetId="10" refreshError="1"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -981,10 +1025,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G24"/>
+  <dimension ref="A1:G25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E29" sqref="E29"/>
+      <selection activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1020,12 +1064,12 @@
       </c>
       <c r="F3" s="2" t="str">
         <f>A4</f>
-        <v>CH12 3456 7890 1234 5678 9</v>
+        <v>CH58 0079 1123 0008 8901 2</v>
       </c>
     </row>
     <row r="4" spans="1:7" s="7" customFormat="1" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A4" s="7" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="B4" s="5"/>
       <c r="F4" s="2" t="str">
@@ -1035,7 +1079,7 @@
     </row>
     <row r="5" spans="1:7" s="1" customFormat="1" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A5" s="7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B5" s="2"/>
       <c r="F5" s="2" t="str">
@@ -1045,7 +1089,7 @@
     </row>
     <row r="6" spans="1:7" s="1" customFormat="1" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A6" s="7" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B6" s="2"/>
       <c r="F6" s="2" t="str">
@@ -1069,22 +1113,22 @@
         <v>5</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="10" spans="1:7" s="1" customFormat="1" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A10" s="7" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B10" s="5"/>
       <c r="F10" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G10" s="8"/>
     </row>
     <row r="11" spans="1:7" s="1" customFormat="1" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A11" s="9" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B11" s="2"/>
     </row>
@@ -1145,47 +1189,48 @@
         <v>123.45</v>
       </c>
     </row>
-    <row r="17" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A17" s="12"/>
-      <c r="B17" s="12"/>
-      <c r="C17"/>
-      <c r="D17"/>
-      <c r="E17"/>
+    <row r="17" spans="1:6" s="1" customFormat="1" ht="13.5" x14ac:dyDescent="0.35">
+      <c r="A17" s="7"/>
+      <c r="B17" s="10"/>
+      <c r="D17" s="2"/>
+      <c r="E17" s="11"/>
     </row>
     <row r="18" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A18" s="12"/>
-      <c r="B18" s="12"/>
+      <c r="B18"/>
       <c r="C18" s="13" t="s">
         <v>9</v>
       </c>
       <c r="D18"/>
-      <c r="E18"/>
-      <c r="F18" s="2"/>
-    </row>
-    <row r="19" spans="1:6" s="1" customFormat="1" ht="13.5" x14ac:dyDescent="0.35">
+    </row>
+    <row r="19" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="B19" s="12"/>
+      <c r="D19"/>
+      <c r="E19"/>
       <c r="F19" s="2"/>
+    </row>
+    <row r="20" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A20"/>
+      <c r="F20" s="2"/>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A22" s="12"/>
-      <c r="B22" s="12"/>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A23" s="12"/>
       <c r="B23" s="12"/>
     </row>
-    <row r="24" spans="1:6" s="15" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A24" s="15" t="s">
-        <v>17</v>
-      </c>
-      <c r="F24" s="16"/>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A24" s="15"/>
+      <c r="B24" s="12"/>
+    </row>
+    <row r="25" spans="1:6" s="15" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A25"/>
+      <c r="F25" s="16"/>
     </row>
   </sheetData>
-  <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A17:B17" xr:uid="{93FBC89B-9ED8-4C94-A9A4-8FCA9ECA92CF}">
-      <formula1>NameAusAdressdaten</formula1>
-    </dataValidation>
-  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added a ribbon button.
</commit_message>
<xml_diff>
--- a/SwissQRBill.xlsx
+++ b/SwissQRBill.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23001"/>
   <workbookPr filterPrivacy="1" checkCompatibility="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46724573-5DA6-4E3A-A9BA-09AAF1239974}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD42654F-3365-4E46-9548-8D0F199B67B6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15796" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -92,7 +92,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="14" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -141,12 +141,6 @@
     </font>
     <font>
       <sz val="8"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="9"/>
       <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
@@ -221,18 +215,20 @@
     <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -314,7 +310,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>668660</xdr:colOff>
+      <xdr:colOff>592460</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>47625</xdr:rowOff>
     </xdr:to>
@@ -332,7 +328,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="4760" y="38088"/>
-          <a:ext cx="7636200" cy="9537"/>
+          <a:ext cx="7560000" cy="9537"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -363,7 +359,7 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>21</xdr:row>
-      <xdr:rowOff>80960</xdr:rowOff>
+      <xdr:rowOff>90488</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
@@ -384,8 +380,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="0" y="3795710"/>
-          <a:ext cx="2232000" cy="9537"/>
+          <a:off x="0" y="3805238"/>
+          <a:ext cx="2232000" cy="9"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -420,9 +416,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>594119</xdr:colOff>
+      <xdr:colOff>585788</xdr:colOff>
       <xdr:row>21</xdr:row>
-      <xdr:rowOff>100022</xdr:rowOff>
+      <xdr:rowOff>90488</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -438,7 +434,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="2238419" y="3805235"/>
-          <a:ext cx="5328000" cy="9537"/>
+          <a:ext cx="5319669" cy="3"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -691,10 +687,10 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="8" name="Picture 7">
+        <xdr:cNvPr id="10" name="Picture 9">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B1A84A10-63C5-4A08-9FF2-3528FF80C16C}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{416FAD65-3211-46CD-8E59-825638C8BB1A}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -739,6 +735,7 @@
       <sheetName val="Selbst Säck"/>
       <sheetName val="KK Säck"/>
       <sheetName val="KK Basel"/>
+      <sheetName val="QR Rechnung Basel"/>
       <sheetName val="Pivot Rechnungsnummern"/>
       <sheetName val="Auswertungen pro Mo"/>
       <sheetName val="Listen"/>
@@ -746,17 +743,18 @@
       <sheetName val="RECHNUNGSWESEN für QR"/>
     </sheetNames>
     <sheetDataSet>
-      <sheetData sheetId="0" refreshError="1"/>
+      <sheetData sheetId="0"/>
       <sheetData sheetId="1"/>
-      <sheetData sheetId="2" refreshError="1"/>
-      <sheetData sheetId="3" refreshError="1"/>
-      <sheetData sheetId="4" refreshError="1"/>
-      <sheetData sheetId="5" refreshError="1"/>
-      <sheetData sheetId="6" refreshError="1"/>
-      <sheetData sheetId="7" refreshError="1"/>
-      <sheetData sheetId="8" refreshError="1"/>
-      <sheetData sheetId="9" refreshError="1"/>
-      <sheetData sheetId="10" refreshError="1"/>
+      <sheetData sheetId="2"/>
+      <sheetData sheetId="3"/>
+      <sheetData sheetId="4"/>
+      <sheetData sheetId="5"/>
+      <sheetData sheetId="6"/>
+      <sheetData sheetId="7"/>
+      <sheetData sheetId="8"/>
+      <sheetData sheetId="9"/>
+      <sheetData sheetId="10"/>
+      <sheetData sheetId="11" refreshError="1"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -1028,7 +1026,7 @@
   <dimension ref="A1:G25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A24" sqref="A24"/>
+      <selection activeCell="G30" sqref="G30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1038,7 +1036,7 @@
     <col min="3" max="3" width="17.19921875" customWidth="1"/>
     <col min="4" max="4" width="8.59765625" customWidth="1"/>
     <col min="5" max="5" width="17.1328125" customWidth="1"/>
-    <col min="6" max="6" width="10.6640625" style="14"/>
+    <col min="6" max="6" width="10.6640625" style="13"/>
     <col min="7" max="7" width="17.06640625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1102,8 +1100,10 @@
         <v>3</v>
       </c>
       <c r="B7" s="2"/>
+      <c r="F7" s="2"/>
     </row>
     <row r="8" spans="1:7" s="1" customFormat="1" ht="13.5" x14ac:dyDescent="0.35">
+      <c r="A8" s="7"/>
       <c r="F8" s="5" t="s">
         <v>4</v>
       </c>
@@ -1127,10 +1127,11 @@
       <c r="G10" s="8"/>
     </row>
     <row r="11" spans="1:7" s="1" customFormat="1" ht="13.5" x14ac:dyDescent="0.35">
-      <c r="A11" s="9" t="s">
+      <c r="A11" s="7" t="s">
         <v>13</v>
       </c>
       <c r="B11" s="2"/>
+      <c r="F11" s="2"/>
     </row>
     <row r="12" spans="1:7" s="1" customFormat="1" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A12" s="7" t="s">
@@ -1142,6 +1143,7 @@
       </c>
     </row>
     <row r="13" spans="1:7" s="1" customFormat="1" ht="13.5" x14ac:dyDescent="0.35">
+      <c r="A13" s="7"/>
       <c r="B13" s="5"/>
       <c r="F13" s="2" t="str">
         <f>A10</f>
@@ -1149,6 +1151,7 @@
       </c>
     </row>
     <row r="14" spans="1:7" s="1" customFormat="1" ht="13.5" x14ac:dyDescent="0.35">
+      <c r="A14" s="7"/>
       <c r="B14" s="2"/>
       <c r="F14" s="2" t="str">
         <f>A11</f>
@@ -1177,34 +1180,37 @@
       <c r="A16" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="B16" s="10">
+      <c r="B16" s="9">
         <v>123.45</v>
       </c>
       <c r="D16" s="2" t="str">
         <f>A16</f>
         <v>CHF</v>
       </c>
-      <c r="E16" s="11">
+      <c r="E16" s="16">
         <f>B16</f>
         <v>123.45</v>
       </c>
+      <c r="F16" s="2"/>
     </row>
     <row r="17" spans="1:6" s="1" customFormat="1" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A17" s="7"/>
-      <c r="B17" s="10"/>
+      <c r="B17" s="9"/>
       <c r="D17" s="2"/>
-      <c r="E17" s="11"/>
+      <c r="E17" s="10"/>
+      <c r="F17" s="2"/>
     </row>
     <row r="18" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A18" s="12"/>
+      <c r="A18" s="11"/>
       <c r="B18"/>
-      <c r="C18" s="13" t="s">
+      <c r="C18" s="12" t="s">
         <v>9</v>
       </c>
       <c r="D18"/>
+      <c r="F18" s="2"/>
     </row>
     <row r="19" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="B19" s="12"/>
+      <c r="B19" s="11"/>
       <c r="D19"/>
       <c r="E19"/>
       <c r="F19" s="2"/>
@@ -1214,19 +1220,19 @@
       <c r="F20" s="2"/>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A22" s="12"/>
+      <c r="A22" s="11"/>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A23" s="12"/>
-      <c r="B23" s="12"/>
+      <c r="A23" s="11"/>
+      <c r="B23" s="11"/>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A24" s="15"/>
-      <c r="B24" s="12"/>
-    </row>
-    <row r="25" spans="1:6" s="15" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A24" s="14"/>
+      <c r="B24" s="11"/>
+    </row>
+    <row r="25" spans="1:6" s="14" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A25"/>
-      <c r="F25" s="16"/>
+      <c r="F25" s="15"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Small update to template.
</commit_message>
<xml_diff>
--- a/SwissQRBill.xlsx
+++ b/SwissQRBill.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23001"/>
   <workbookPr filterPrivacy="1" checkCompatibility="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD42654F-3365-4E46-9548-8D0F199B67B6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F02E67A-C43C-45AB-9212-F520271F00D4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15796" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -670,56 +670,6 @@
         </a:fontRef>
       </xdr:style>
     </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>1123950</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>79375</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>1058862</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>152400</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="10" name="Picture 9">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{416FAD65-3211-46CD-8E59-825638C8BB1A}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="2286000" y="508000"/>
-          <a:ext cx="1778000" cy="1778000"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>

</xml_diff>